<commit_message>
Updated codes for read and write in excel.
</commit_message>
<xml_diff>
--- a/18-03-2021/Demo.xlsx
+++ b/18-03-2021/Demo.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17970" windowHeight="5940" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17970" windowHeight="5940" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -17,14 +17,13 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
     <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
     <sheet name="Sheet5" sheetId="5" r:id="rId5"/>
-    <sheet name="mastersheet" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="86">
   <si>
     <t>PS number</t>
   </si>
@@ -725,8 +724,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B41"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1073,8 +1072,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B41"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1421,8 +1420,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B41"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1453,7 +1452,7 @@
       </c>
       <c r="B3">
         <f t="shared" ref="B3:B30" ca="1" si="0">RANDBETWEEN(10000000,99999999)</f>
-        <v>75560504</v>
+        <v>33734590</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -1462,7 +1461,7 @@
       </c>
       <c r="B4">
         <f t="shared" ca="1" si="0"/>
-        <v>11444478</v>
+        <v>66480027</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -1471,7 +1470,7 @@
       </c>
       <c r="B5">
         <f t="shared" ca="1" si="0"/>
-        <v>35441840</v>
+        <v>49275863</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -1480,7 +1479,7 @@
       </c>
       <c r="B6">
         <f t="shared" ca="1" si="0"/>
-        <v>18318073</v>
+        <v>48588487</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -1489,7 +1488,7 @@
       </c>
       <c r="B7">
         <f t="shared" ca="1" si="0"/>
-        <v>92204204</v>
+        <v>64621726</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -1498,7 +1497,7 @@
       </c>
       <c r="B8">
         <f t="shared" ca="1" si="0"/>
-        <v>40151609</v>
+        <v>91797229</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -1507,7 +1506,7 @@
       </c>
       <c r="B9">
         <f t="shared" ca="1" si="0"/>
-        <v>95371891</v>
+        <v>39805885</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -1516,7 +1515,7 @@
       </c>
       <c r="B10">
         <f t="shared" ca="1" si="0"/>
-        <v>98662760</v>
+        <v>95388440</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -1525,7 +1524,7 @@
       </c>
       <c r="B11">
         <f t="shared" ca="1" si="0"/>
-        <v>16453086</v>
+        <v>12825092</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -1534,7 +1533,7 @@
       </c>
       <c r="B12">
         <f t="shared" ca="1" si="0"/>
-        <v>89994415</v>
+        <v>29445199</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -1543,7 +1542,7 @@
       </c>
       <c r="B13">
         <f t="shared" ca="1" si="0"/>
-        <v>96089828</v>
+        <v>22386198</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -1552,7 +1551,7 @@
       </c>
       <c r="B14">
         <f t="shared" ca="1" si="0"/>
-        <v>38627074</v>
+        <v>80914988</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
@@ -1561,7 +1560,7 @@
       </c>
       <c r="B15">
         <f t="shared" ca="1" si="0"/>
-        <v>88738337</v>
+        <v>50079745</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
@@ -1570,7 +1569,7 @@
       </c>
       <c r="B16">
         <f t="shared" ca="1" si="0"/>
-        <v>99967106</v>
+        <v>37419642</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -1579,7 +1578,7 @@
       </c>
       <c r="B17">
         <f t="shared" ca="1" si="0"/>
-        <v>99445146</v>
+        <v>73579280</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
@@ -1588,7 +1587,7 @@
       </c>
       <c r="B18">
         <f t="shared" ca="1" si="0"/>
-        <v>47412973</v>
+        <v>17221814</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -1597,7 +1596,7 @@
       </c>
       <c r="B19">
         <f t="shared" ca="1" si="0"/>
-        <v>73960837</v>
+        <v>86112259</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
@@ -1606,7 +1605,7 @@
       </c>
       <c r="B20">
         <f t="shared" ca="1" si="0"/>
-        <v>93983255</v>
+        <v>73340524</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
@@ -1615,7 +1614,7 @@
       </c>
       <c r="B21">
         <f t="shared" ca="1" si="0"/>
-        <v>73169086</v>
+        <v>99845336</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
@@ -1624,7 +1623,7 @@
       </c>
       <c r="B22">
         <f t="shared" ca="1" si="0"/>
-        <v>61419412</v>
+        <v>53900461</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
@@ -1633,7 +1632,7 @@
       </c>
       <c r="B23">
         <f t="shared" ca="1" si="0"/>
-        <v>33330154</v>
+        <v>42999098</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
@@ -1642,7 +1641,7 @@
       </c>
       <c r="B24">
         <f t="shared" ca="1" si="0"/>
-        <v>77693716</v>
+        <v>18492594</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
@@ -1651,7 +1650,7 @@
       </c>
       <c r="B25">
         <f t="shared" ca="1" si="0"/>
-        <v>67413634</v>
+        <v>69573520</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
@@ -1660,7 +1659,7 @@
       </c>
       <c r="B26">
         <f t="shared" ca="1" si="0"/>
-        <v>86727754</v>
+        <v>88519022</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
@@ -1669,7 +1668,7 @@
       </c>
       <c r="B27">
         <f t="shared" ca="1" si="0"/>
-        <v>56444149</v>
+        <v>51434911</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
@@ -1678,7 +1677,7 @@
       </c>
       <c r="B28">
         <f t="shared" ca="1" si="0"/>
-        <v>23212307</v>
+        <v>92513590</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
@@ -1687,7 +1686,7 @@
       </c>
       <c r="B29">
         <f t="shared" ca="1" si="0"/>
-        <v>30578088</v>
+        <v>72612386</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
@@ -1696,7 +1695,7 @@
       </c>
       <c r="B30">
         <f t="shared" ca="1" si="0"/>
-        <v>72002022</v>
+        <v>78232843</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
@@ -1713,7 +1712,7 @@
       </c>
       <c r="B32">
         <f t="shared" ref="B32:B41" ca="1" si="1">RANDBETWEEN(10000000,99999999)</f>
-        <v>80129836</v>
+        <v>68970285</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
@@ -1722,7 +1721,7 @@
       </c>
       <c r="B33">
         <f t="shared" ca="1" si="1"/>
-        <v>18833387</v>
+        <v>92409664</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
@@ -1731,7 +1730,7 @@
       </c>
       <c r="B34">
         <f t="shared" ca="1" si="1"/>
-        <v>78789621</v>
+        <v>74684643</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
@@ -1740,7 +1739,7 @@
       </c>
       <c r="B35">
         <f t="shared" ca="1" si="1"/>
-        <v>86358653</v>
+        <v>82252866</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
@@ -1749,7 +1748,7 @@
       </c>
       <c r="B36">
         <f t="shared" ca="1" si="1"/>
-        <v>85958032</v>
+        <v>47123581</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
@@ -1758,7 +1757,7 @@
       </c>
       <c r="B37">
         <f t="shared" ca="1" si="1"/>
-        <v>31769269</v>
+        <v>47099522</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
@@ -1767,7 +1766,7 @@
       </c>
       <c r="B38">
         <f t="shared" ca="1" si="1"/>
-        <v>85056360</v>
+        <v>73668282</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
@@ -1776,7 +1775,7 @@
       </c>
       <c r="B39">
         <f t="shared" ca="1" si="1"/>
-        <v>56482831</v>
+        <v>76399179</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
@@ -1785,7 +1784,7 @@
       </c>
       <c r="B40">
         <f t="shared" ca="1" si="1"/>
-        <v>55841076</v>
+        <v>45038620</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
@@ -1794,7 +1793,7 @@
       </c>
       <c r="B41">
         <f t="shared" ca="1" si="1"/>
-        <v>22475225</v>
+        <v>15011398</v>
       </c>
     </row>
   </sheetData>
@@ -1807,8 +1806,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B41"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1831,7 +1830,7 @@
       </c>
       <c r="B2">
         <f t="shared" ref="B2:B14" ca="1" si="0">RANDBETWEEN(5000,11000)</f>
-        <v>6708</v>
+        <v>7945</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1840,7 +1839,7 @@
       </c>
       <c r="B3">
         <f t="shared" ca="1" si="0"/>
-        <v>8980</v>
+        <v>8037</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -1849,7 +1848,7 @@
       </c>
       <c r="B4">
         <f t="shared" ca="1" si="0"/>
-        <v>6951</v>
+        <v>8759</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -1858,7 +1857,7 @@
       </c>
       <c r="B5">
         <f t="shared" ca="1" si="0"/>
-        <v>8921</v>
+        <v>7510</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -1867,7 +1866,7 @@
       </c>
       <c r="B6">
         <f t="shared" ca="1" si="0"/>
-        <v>10340</v>
+        <v>5592</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -1876,7 +1875,7 @@
       </c>
       <c r="B7">
         <f t="shared" ca="1" si="0"/>
-        <v>10365</v>
+        <v>7045</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -1885,7 +1884,7 @@
       </c>
       <c r="B8">
         <f t="shared" ca="1" si="0"/>
-        <v>8428</v>
+        <v>9605</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -1894,7 +1893,7 @@
       </c>
       <c r="B9">
         <f t="shared" ca="1" si="0"/>
-        <v>6166</v>
+        <v>8627</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -1903,7 +1902,7 @@
       </c>
       <c r="B10">
         <f t="shared" ca="1" si="0"/>
-        <v>8150</v>
+        <v>8672</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -1912,7 +1911,7 @@
       </c>
       <c r="B11">
         <f t="shared" ca="1" si="0"/>
-        <v>10481</v>
+        <v>10025</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -1921,7 +1920,7 @@
       </c>
       <c r="B12">
         <f t="shared" ca="1" si="0"/>
-        <v>10211</v>
+        <v>8446</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -1930,7 +1929,7 @@
       </c>
       <c r="B13">
         <f t="shared" ca="1" si="0"/>
-        <v>7436</v>
+        <v>7056</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -1939,7 +1938,7 @@
       </c>
       <c r="B14">
         <f t="shared" ca="1" si="0"/>
-        <v>7981</v>
+        <v>10354</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
@@ -1956,7 +1955,7 @@
       </c>
       <c r="B16">
         <f t="shared" ref="B16:B30" ca="1" si="1">RANDBETWEEN(5000,11000)</f>
-        <v>7999</v>
+        <v>8872</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -1965,7 +1964,7 @@
       </c>
       <c r="B17">
         <f t="shared" ca="1" si="1"/>
-        <v>5406</v>
+        <v>6990</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
@@ -1974,7 +1973,7 @@
       </c>
       <c r="B18">
         <f t="shared" ca="1" si="1"/>
-        <v>8345</v>
+        <v>9124</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -1983,7 +1982,7 @@
       </c>
       <c r="B19">
         <f t="shared" ca="1" si="1"/>
-        <v>8958</v>
+        <v>7387</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
@@ -1992,7 +1991,7 @@
       </c>
       <c r="B20">
         <f t="shared" ca="1" si="1"/>
-        <v>8519</v>
+        <v>9757</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
@@ -2001,7 +2000,7 @@
       </c>
       <c r="B21">
         <f t="shared" ca="1" si="1"/>
-        <v>6696</v>
+        <v>7535</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
@@ -2010,7 +2009,7 @@
       </c>
       <c r="B22">
         <f t="shared" ca="1" si="1"/>
-        <v>5188</v>
+        <v>10035</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
@@ -2019,7 +2018,7 @@
       </c>
       <c r="B23">
         <f t="shared" ca="1" si="1"/>
-        <v>10493</v>
+        <v>8639</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
@@ -2028,7 +2027,7 @@
       </c>
       <c r="B24">
         <f t="shared" ca="1" si="1"/>
-        <v>8680</v>
+        <v>6565</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
@@ -2037,7 +2036,7 @@
       </c>
       <c r="B25">
         <f t="shared" ca="1" si="1"/>
-        <v>7883</v>
+        <v>8662</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
@@ -2046,7 +2045,7 @@
       </c>
       <c r="B26">
         <f t="shared" ca="1" si="1"/>
-        <v>6683</v>
+        <v>8505</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
@@ -2055,7 +2054,7 @@
       </c>
       <c r="B27">
         <f t="shared" ca="1" si="1"/>
-        <v>7731</v>
+        <v>7227</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
@@ -2064,7 +2063,7 @@
       </c>
       <c r="B28">
         <f t="shared" ca="1" si="1"/>
-        <v>5328</v>
+        <v>5123</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
@@ -2073,7 +2072,7 @@
       </c>
       <c r="B29">
         <f t="shared" ca="1" si="1"/>
-        <v>8947</v>
+        <v>8643</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
@@ -2082,7 +2081,7 @@
       </c>
       <c r="B30">
         <f t="shared" ca="1" si="1"/>
-        <v>8950</v>
+        <v>10844</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
@@ -2099,7 +2098,7 @@
       </c>
       <c r="B32">
         <f t="shared" ref="B32:B41" ca="1" si="2">RANDBETWEEN(5000,11000)</f>
-        <v>7161</v>
+        <v>8197</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
@@ -2108,7 +2107,7 @@
       </c>
       <c r="B33">
         <f t="shared" ca="1" si="2"/>
-        <v>8606</v>
+        <v>6185</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
@@ -2117,7 +2116,7 @@
       </c>
       <c r="B34">
         <f t="shared" ca="1" si="2"/>
-        <v>5708</v>
+        <v>10941</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
@@ -2126,7 +2125,7 @@
       </c>
       <c r="B35">
         <f t="shared" ca="1" si="2"/>
-        <v>9204</v>
+        <v>5640</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
@@ -2135,7 +2134,7 @@
       </c>
       <c r="B36">
         <f t="shared" ca="1" si="2"/>
-        <v>9703</v>
+        <v>5341</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
@@ -2144,7 +2143,7 @@
       </c>
       <c r="B37">
         <f t="shared" ca="1" si="2"/>
-        <v>5145</v>
+        <v>9866</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
@@ -2153,7 +2152,7 @@
       </c>
       <c r="B38">
         <f t="shared" ca="1" si="2"/>
-        <v>9557</v>
+        <v>9456</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
@@ -2162,7 +2161,7 @@
       </c>
       <c r="B39">
         <f t="shared" ca="1" si="2"/>
-        <v>8537</v>
+        <v>10749</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
@@ -2171,7 +2170,7 @@
       </c>
       <c r="B40">
         <f t="shared" ca="1" si="2"/>
-        <v>6091</v>
+        <v>7798</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
@@ -2180,7 +2179,7 @@
       </c>
       <c r="B41">
         <f t="shared" ca="1" si="2"/>
-        <v>9744</v>
+        <v>8553</v>
       </c>
     </row>
   </sheetData>
@@ -2193,8 +2192,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B41"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2577,99 +2576,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B10"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1">
-        <v>99003772</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3">
-        <v>99003772</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>42</v>
-      </c>
-      <c r="B4">
-        <v>344421</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B5">
-        <v>99003772</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>43</v>
-      </c>
-      <c r="B6">
-        <f ca="1">RANDBETWEEN(10000000,99999999)</f>
-        <v>60969549</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>0</v>
-      </c>
-      <c r="B7">
-        <v>99003772</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>44</v>
-      </c>
-      <c r="B8">
-        <f ca="1">RANDBETWEEN(5000,11000)</f>
-        <v>10354</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>0</v>
-      </c>
-      <c r="B9">
-        <v>99003772</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>45</v>
-      </c>
-      <c r="B10" t="s">
-        <v>71</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
 </file>
</xml_diff>